<commit_message>
(#139) Fix error parsing compositions with 1:1
</commit_message>
<xml_diff>
--- a/test/data/xlsx/Packungen-2019.01.31.xlsx
+++ b/test/data/xlsx/Packungen-2019.01.31.xlsx
@@ -12,16 +12,6 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Zugelassene Packungen'!$6:$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Zugelassene Packungen'!$6:$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">'Zugelassene Packungen'!$6:$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'Zugelassene Packungen'!$6:$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">'Zugelassene Packungen'!$6:$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0" vbProcedure="false">'Zugelassene Packungen'!$6:$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0" vbProcedure="false">'Zugelassene Packungen'!$6:$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0" vbProcedure="false">'Zugelassene Packungen'!$6:$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0" vbProcedure="false">'Zugelassene Packungen'!$6:$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0" vbProcedure="false">'Zugelassene Packungen'!$6:$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Zugelassene Packungen'!$6:$6</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -33,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="304">
   <si>
     <t xml:space="preserve">Zugelassene Packungen Humanarzneimittel </t>
   </si>
@@ -955,12 +945,6 @@
   </si>
   <si>
     <t xml:space="preserve">L01XX46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016/01/14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021/01/13</t>
   </si>
   <si>
     <t xml:space="preserve">4 x 112</t>
@@ -1435,13 +1419,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1517,9 +1501,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>442800</xdr:colOff>
+      <xdr:colOff>442440</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>35280</xdr:rowOff>
+      <xdr:rowOff>34920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1533,7 +1517,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="36360" y="360"/>
-          <a:ext cx="1682640" cy="568080"/>
+          <a:ext cx="1682280" cy="567720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1554,9 +1538,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>246960</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>48600</xdr:rowOff>
+      <xdr:rowOff>48240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1570,7 +1554,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5400" y="9360"/>
-          <a:ext cx="946080" cy="572400"/>
+          <a:ext cx="945720" cy="572040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1593,12 +1577,12 @@
   <dimension ref="A1:AMJ47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="5" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+      <selection pane="bottomLeft" activeCell="J42" activeCellId="0" sqref="J42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="5.9921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="7.39"/>
@@ -1625,7 +1609,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="7" width="7.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="7" width="14.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="7" width="7.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="33" style="7" width="6"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="33" style="7" width="6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22092,23 +22076,23 @@
       <c r="G42" s="0" t="s">
         <v>280</v>
       </c>
-      <c r="H42" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="I42" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="J42" s="0" t="s">
-        <v>282</v>
+      <c r="H42" s="49" t="n">
+        <v>42513</v>
+      </c>
+      <c r="I42" s="49" t="n">
+        <v>42513</v>
+      </c>
+      <c r="J42" s="49" t="n">
+        <v>42513</v>
       </c>
       <c r="K42" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L42" s="0" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M42" s="0" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="N42" s="0" t="s">
         <v>122</v>
@@ -22120,14 +22104,14 @@
         <v>122</v>
       </c>
       <c r="Q42" s="0" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="R42" s="0" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="S42" s="0"/>
       <c r="T42" s="0" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="U42" s="0"/>
       <c r="V42" s="0"/>
@@ -23141,10 +23125,10 @@
         <v>1</v>
       </c>
       <c r="C43" s="39" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D43" s="39" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E43" s="40" t="s">
         <v>218</v>
@@ -23153,7 +23137,7 @@
         <v>219</v>
       </c>
       <c r="G43" s="40" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H43" s="41" t="n">
         <v>39296</v>
@@ -23183,14 +23167,14 @@
         <v>36</v>
       </c>
       <c r="Q43" s="39" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="R43" s="39" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="S43" s="39"/>
       <c r="T43" s="39" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="U43" s="39"/>
       <c r="V43" s="40"/>
@@ -24204,19 +24188,19 @@
         <v>1</v>
       </c>
       <c r="C44" s="39" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D44" s="39" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E44" s="40" t="s">
         <v>44</v>
       </c>
       <c r="F44" s="40" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G44" s="40" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H44" s="41" t="n">
         <v>29980</v>
@@ -24231,7 +24215,7 @@
         <v>29</v>
       </c>
       <c r="L44" s="37" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M44" s="39" t="s">
         <v>48</v>
@@ -24246,14 +24230,14 @@
         <v>36</v>
       </c>
       <c r="Q44" s="39" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="R44" s="39" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="S44" s="39"/>
       <c r="T44" s="39" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="U44" s="39"/>
       <c r="V44" s="40"/>
@@ -26330,19 +26314,19 @@
         <v>1</v>
       </c>
       <c r="C46" s="39" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D46" s="39" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E46" s="40" t="s">
         <v>44</v>
       </c>
       <c r="F46" s="40" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G46" s="40" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H46" s="41" t="n">
         <v>27529</v>
@@ -26372,14 +26356,14 @@
         <v>36</v>
       </c>
       <c r="Q46" s="39" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="R46" s="39" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="S46" s="39"/>
       <c r="T46" s="39" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="U46" s="39"/>
       <c r="V46" s="40"/>
@@ -27393,19 +27377,19 @@
         <v>1</v>
       </c>
       <c r="C47" s="39" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D47" s="39" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E47" s="40" t="s">
         <v>44</v>
       </c>
       <c r="F47" s="40" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G47" s="40" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H47" s="41" t="n">
         <v>27529</v>
@@ -27420,7 +27404,7 @@
         <v>58</v>
       </c>
       <c r="L47" s="37" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="M47" s="39" t="s">
         <v>48</v>
@@ -27435,14 +27419,14 @@
         <v>36</v>
       </c>
       <c r="Q47" s="39" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="R47" s="39" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="S47" s="39"/>
       <c r="T47" s="39" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="U47" s="39"/>
       <c r="V47" s="40"/>

</xml_diff>